<commit_message>
Restructured database and updated GUIs
Added ID field to database, moved position of Notes column. 
Current Order GUI can now update entries in the database with time of completion and a completion code (completion codes found in constants)
Automated function calls for importing from database, updating orders, resetting fields, etc on both GUIs
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kyle\Desktop\osrs_flip_helper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\file_sys\work\workspace\osrs_stocks_12_3\osrs_stocks-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4B972F-1299-4724-85D4-EDCDCAB2E716}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68546567-1761-4FA4-9E38-B61EF65DD918}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12684" yWindow="6216" windowWidth="10356" windowHeight="6132" xr2:uid="{3A4BCD19-BC7F-46D6-80EE-26271915C7B0}"/>
+    <workbookView xWindow="47880" yWindow="2655" windowWidth="24240" windowHeight="13140" xr2:uid="{3A4BCD19-BC7F-46D6-80EE-26271915C7B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="68">
   <si>
     <t>Shark</t>
   </si>
@@ -191,6 +191,51 @@
   </si>
   <si>
     <t>Papaya fruit</t>
+  </si>
+  <si>
+    <t>Water orb</t>
+  </si>
+  <si>
+    <t>Earth orb</t>
+  </si>
+  <si>
+    <t>Bandos dragonhide set</t>
+  </si>
+  <si>
+    <t>Saradomin brew(4)</t>
+  </si>
+  <si>
+    <t>Dinh's bulwark</t>
+  </si>
+  <si>
+    <t>Cooked karambwan</t>
+  </si>
+  <si>
+    <t>Ring of 3rd age</t>
+  </si>
+  <si>
+    <t>Divine ranging potion (2)</t>
+  </si>
+  <si>
+    <t>Toktz-xil-ak</t>
+  </si>
+  <si>
+    <t>Xerician robe</t>
+  </si>
+  <si>
+    <t>Snape grass seed</t>
+  </si>
+  <si>
+    <t>3rd age range coif</t>
+  </si>
+  <si>
+    <t>Toxic blowpipe (empty)</t>
+  </si>
+  <si>
+    <t>Wyrm bones</t>
+  </si>
+  <si>
+    <t>Ancient d'hide boots</t>
   </si>
 </sst>
 </file>
@@ -565,20 +610,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAF0EA10-1A19-4FED-AAA3-974607F1F301}">
-  <dimension ref="A1:M88"/>
+  <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -619,7 +664,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -644,28 +689,28 @@
         <v>19</v>
       </c>
       <c r="H2">
-        <v>466</v>
+        <v>1664</v>
       </c>
       <c r="I2">
-        <v>479</v>
+        <v>1681</v>
       </c>
       <c r="J2" s="5">
-        <v>10</v>
+        <v>7.5</v>
       </c>
       <c r="K2">
         <f>I2-H2</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="L2">
         <f>(I2*J2-H2*J2)/(H2*J2) *100</f>
-        <v>2.7896995708154506</v>
+        <v>1.0216346153846154</v>
       </c>
       <c r="M2">
         <f>K2*J2</f>
-        <v>130</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -690,7 +735,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -718,7 +763,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -743,11 +788,11 @@
         <v>19</v>
       </c>
       <c r="H5">
-        <f>SUM(F2:F98)</f>
-        <v>11157.156000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+        <f>SUM(F2:F94)</f>
+        <v>17549.015000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -772,7 +817,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -797,7 +842,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -822,7 +867,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -847,7 +892,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -872,7 +917,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -897,7 +942,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -922,7 +967,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -947,7 +992,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -972,7 +1017,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -997,7 +1042,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1022,7 +1067,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1047,7 +1092,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -1072,7 +1117,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -1097,7 +1142,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1122,7 +1167,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1147,7 +1192,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -1172,7 +1217,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -1197,7 +1242,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1222,7 +1267,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -1247,7 +1292,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -1272,7 +1317,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -1297,7 +1342,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -1322,7 +1367,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1347,7 +1392,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1372,7 +1417,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>44</v>
       </c>
@@ -1397,7 +1442,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>45</v>
       </c>
@@ -1422,7 +1467,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -1447,7 +1492,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>25</v>
       </c>
@@ -1472,7 +1517,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -1490,14 +1535,14 @@
         <v>28996</v>
       </c>
       <c r="F35" s="4">
-        <f t="shared" ref="F35:F59" si="5">E35*D35</f>
+        <f t="shared" ref="F35:F58" si="5">E35*D35</f>
         <v>202.97200000000001</v>
       </c>
       <c r="G35" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>20</v>
       </c>
@@ -1522,7 +1567,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>31</v>
       </c>
@@ -1547,7 +1592,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1572,7 +1617,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1597,7 +1642,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>27</v>
       </c>
@@ -1622,7 +1667,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -1647,7 +1692,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>37</v>
       </c>
@@ -1672,7 +1717,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>48</v>
       </c>
@@ -1697,7 +1742,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>25</v>
       </c>
@@ -1722,7 +1767,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -1747,7 +1792,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>20</v>
       </c>
@@ -1772,7 +1817,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>17</v>
       </c>
@@ -1797,7 +1842,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>50</v>
       </c>
@@ -1822,7 +1867,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>16</v>
       </c>
@@ -1836,7 +1881,7 @@
         <v>7.5</v>
       </c>
       <c r="E49">
-        <f t="shared" ref="E49:E77" si="6">C49-B49</f>
+        <f t="shared" ref="E49:E58" si="6">C49-B49</f>
         <v>34</v>
       </c>
       <c r="F49" s="4">
@@ -1847,7 +1892,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>25</v>
       </c>
@@ -1872,7 +1917,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>20</v>
       </c>
@@ -1897,362 +1942,771 @@
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B52">
-        <v>8108</v>
+        <v>239</v>
       </c>
       <c r="C52">
-        <v>8135</v>
+        <v>241</v>
       </c>
       <c r="D52">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="E52">
         <f t="shared" si="6"/>
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="F52" s="4">
         <f t="shared" si="5"/>
-        <v>81</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="G52" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B53">
-        <v>239</v>
+        <v>306</v>
       </c>
       <c r="C53">
-        <v>241</v>
+        <v>309</v>
       </c>
       <c r="D53">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E53">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F53" s="4">
         <f t="shared" si="5"/>
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="G53" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B54">
-        <v>306</v>
+        <v>630000</v>
       </c>
       <c r="C54">
-        <v>309</v>
+        <v>658574</v>
       </c>
       <c r="D54">
-        <v>10</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="E54">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>28574</v>
       </c>
       <c r="F54" s="4">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>200.018</v>
       </c>
       <c r="G54" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="B55">
-        <v>630000</v>
+        <v>1147</v>
       </c>
       <c r="C55">
-        <v>658574</v>
+        <v>1193</v>
       </c>
       <c r="D55">
-        <v>7.0000000000000001E-3</v>
+        <v>10</v>
       </c>
       <c r="E55">
         <f t="shared" si="6"/>
-        <v>28574</v>
+        <v>46</v>
       </c>
       <c r="F55" s="4">
         <f t="shared" si="5"/>
-        <v>200.018</v>
+        <v>460</v>
       </c>
       <c r="G55" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="B56">
-        <v>1147</v>
+        <v>310500</v>
       </c>
       <c r="C56">
-        <v>1193</v>
+        <v>327000</v>
       </c>
       <c r="D56">
-        <v>10</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="E56">
         <f t="shared" si="6"/>
-        <v>46</v>
+        <v>16500</v>
       </c>
       <c r="F56" s="4">
         <f t="shared" si="5"/>
-        <v>460</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+        <v>247.5</v>
+      </c>
+      <c r="G56" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B57">
-        <v>310500</v>
+        <v>466</v>
       </c>
       <c r="C57">
-        <v>327000</v>
+        <v>474</v>
       </c>
       <c r="D57">
-        <v>1.4999999999999999E-2</v>
+        <v>11</v>
       </c>
       <c r="E57">
         <f t="shared" si="6"/>
-        <v>16500</v>
+        <v>8</v>
       </c>
       <c r="F57" s="4">
         <f t="shared" si="5"/>
-        <v>247.5</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+      <c r="G57" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B58">
-        <v>466</v>
+        <v>1248</v>
       </c>
       <c r="C58">
-        <v>474</v>
+        <v>1274</v>
       </c>
       <c r="D58">
         <v>11</v>
       </c>
       <c r="E58">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="F58" s="4">
         <f t="shared" si="5"/>
+        <v>286</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>64</v>
+      </c>
+      <c r="B59">
+        <v>6107000</v>
+      </c>
+      <c r="C59">
+        <v>6376000</v>
+      </c>
+      <c r="D59">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E59">
+        <f>C59-B59</f>
+        <v>269000</v>
+      </c>
+      <c r="F59" s="4">
+        <f>E59*D59</f>
+        <v>807</v>
+      </c>
+      <c r="G59" t="s">
+        <v>19</v>
+      </c>
+      <c r="H59" s="4"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>63</v>
+      </c>
+      <c r="B60">
+        <v>1825</v>
+      </c>
+      <c r="C60">
+        <v>1990</v>
+      </c>
+      <c r="D60">
+        <v>0.2</v>
+      </c>
+      <c r="E60">
+        <f>C60-B60</f>
+        <v>165</v>
+      </c>
+      <c r="F60" s="4">
+        <f>E60*D60</f>
+        <v>33</v>
+      </c>
+      <c r="G60" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>62</v>
+      </c>
+      <c r="B61">
+        <v>7800</v>
+      </c>
+      <c r="C61">
+        <v>9000</v>
+      </c>
+      <c r="D61">
+        <v>0.12</v>
+      </c>
+      <c r="E61">
+        <f>C61-B61</f>
+        <v>1200</v>
+      </c>
+      <c r="F61" s="4">
+        <f>E61*D61</f>
+        <v>144</v>
+      </c>
+      <c r="G61" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>405000</v>
+      </c>
+      <c r="C62">
+        <v>412000</v>
+      </c>
+      <c r="D62">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="E62">
+        <f>C62-B62</f>
+        <v>7000</v>
+      </c>
+      <c r="F62" s="4">
+        <f>E62*D62</f>
+        <v>245.00000000000003</v>
+      </c>
+      <c r="G62" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>60</v>
+      </c>
+      <c r="B63">
+        <v>2745</v>
+      </c>
+      <c r="C63">
+        <v>2990</v>
+      </c>
+      <c r="D63">
+        <v>2</v>
+      </c>
+      <c r="E63">
+        <f>C63-B63</f>
+        <v>245</v>
+      </c>
+      <c r="F63" s="4">
+        <f>E63*D63</f>
+        <v>490</v>
+      </c>
+      <c r="G63" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>59</v>
+      </c>
+      <c r="B64">
+        <v>4512000</v>
+      </c>
+      <c r="C64">
+        <v>4650000</v>
+      </c>
+      <c r="D64">
+        <v>2E-3</v>
+      </c>
+      <c r="E64">
+        <f>C64-B64</f>
+        <v>138000</v>
+      </c>
+      <c r="F64" s="4">
+        <f>E64*D64</f>
+        <v>276</v>
+      </c>
+      <c r="G64" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>58</v>
+      </c>
+      <c r="B65">
+        <v>627</v>
+      </c>
+      <c r="C65">
+        <v>640</v>
+      </c>
+      <c r="D65">
+        <v>10</v>
+      </c>
+      <c r="E65">
+        <f>C65-B65</f>
+        <v>13</v>
+      </c>
+      <c r="F65" s="4">
+        <f>E65*D65</f>
+        <v>130</v>
+      </c>
+      <c r="G65" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>57</v>
+      </c>
+      <c r="B66">
+        <v>4021000</v>
+      </c>
+      <c r="C66">
+        <v>4084990</v>
+      </c>
+      <c r="D66">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="E66">
+        <f>C66-B66</f>
+        <v>63990</v>
+      </c>
+      <c r="F66" s="4">
+        <f>E66*D66</f>
+        <v>447.93</v>
+      </c>
+      <c r="G66" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>56</v>
+      </c>
+      <c r="B67">
+        <v>4680</v>
+      </c>
+      <c r="C67">
+        <v>4722</v>
+      </c>
+      <c r="D67">
+        <v>2</v>
+      </c>
+      <c r="E67">
+        <f>C67-B67</f>
+        <v>42</v>
+      </c>
+      <c r="F67" s="4">
+        <f>E67*D67</f>
+        <v>84</v>
+      </c>
+      <c r="G67" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>55</v>
+      </c>
+      <c r="B68">
+        <v>487199</v>
+      </c>
+      <c r="C68">
+        <v>512400</v>
+      </c>
+      <c r="D68">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="E68">
+        <f>C68-B68</f>
+        <v>25201</v>
+      </c>
+      <c r="F68" s="4">
+        <f>E68*D68</f>
+        <v>176.40700000000001</v>
+      </c>
+      <c r="G68" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>29</v>
+      </c>
+      <c r="B69">
+        <v>45650</v>
+      </c>
+      <c r="C69">
+        <v>47650</v>
+      </c>
+      <c r="D69">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E69">
+        <f>C69-B69</f>
+        <v>2000</v>
+      </c>
+      <c r="F69" s="4">
+        <f>E69*D69</f>
+        <v>140</v>
+      </c>
+      <c r="G69" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>36</v>
+      </c>
+      <c r="B70">
+        <v>3022</v>
+      </c>
+      <c r="C70">
+        <v>3045</v>
+      </c>
+      <c r="D70">
+        <v>7.5</v>
+      </c>
+      <c r="E70">
+        <f>C70-B70</f>
+        <v>23</v>
+      </c>
+      <c r="F70" s="4">
+        <f>E70*D70</f>
+        <v>172.5</v>
+      </c>
+      <c r="G70" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>38</v>
+      </c>
+      <c r="B71">
+        <v>235</v>
+      </c>
+      <c r="C71">
+        <v>237</v>
+      </c>
+      <c r="D71">
+        <v>30</v>
+      </c>
+      <c r="E71">
+        <f>C71-B71</f>
+        <v>2</v>
+      </c>
+      <c r="F71" s="4">
+        <f>E71*D71</f>
+        <v>60</v>
+      </c>
+      <c r="G71" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>28</v>
+      </c>
+      <c r="B72">
+        <v>894000</v>
+      </c>
+      <c r="C72">
+        <v>944500</v>
+      </c>
+      <c r="D72">
+        <v>2E-3</v>
+      </c>
+      <c r="E72">
+        <f>C72-B72</f>
+        <v>50500</v>
+      </c>
+      <c r="F72" s="4">
+        <f>E72*D72</f>
+        <v>101</v>
+      </c>
+      <c r="G72" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>49</v>
+      </c>
+      <c r="B73">
+        <v>1030000</v>
+      </c>
+      <c r="C73">
+        <v>1040000</v>
+      </c>
+      <c r="D73">
+        <v>1.4E-2</v>
+      </c>
+      <c r="E73">
+        <f>C73-B73</f>
+        <v>10000</v>
+      </c>
+      <c r="F73" s="4">
+        <f>E73*D73</f>
+        <v>140</v>
+      </c>
+      <c r="G73" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>64</v>
+      </c>
+      <c r="B74">
+        <v>6180000</v>
+      </c>
+      <c r="C74">
+        <v>6350000</v>
+      </c>
+      <c r="D74">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E74">
+        <f>C74-B74</f>
+        <v>170000</v>
+      </c>
+      <c r="F74" s="4">
+        <f>E74*D74</f>
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>58</v>
+      </c>
+      <c r="B75">
+        <v>633</v>
+      </c>
+      <c r="C75">
+        <v>640</v>
+      </c>
+      <c r="D75">
+        <v>10</v>
+      </c>
+      <c r="E75">
+        <f>C75-B75</f>
+        <v>7</v>
+      </c>
+      <c r="F75" s="4">
+        <f>E75*D75</f>
+        <v>70</v>
+      </c>
+      <c r="G75" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>45</v>
+      </c>
+      <c r="B76">
+        <v>2659</v>
+      </c>
+      <c r="C76">
+        <v>2747</v>
+      </c>
+      <c r="D76">
+        <v>2</v>
+      </c>
+      <c r="E76">
+        <f>C76-B76</f>
         <v>88</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>50</v>
-      </c>
-      <c r="B59">
-        <v>1248</v>
-      </c>
-      <c r="C59">
-        <v>1274</v>
-      </c>
-      <c r="D59">
-        <v>11</v>
-      </c>
-      <c r="E59">
-        <f t="shared" si="6"/>
-        <v>26</v>
-      </c>
-      <c r="F59" s="4">
-        <f t="shared" si="5"/>
-        <v>286</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E60">
-        <f t="shared" si="6"/>
+      <c r="F76" s="4">
+        <f>E76*D76</f>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>65</v>
+      </c>
+      <c r="B77">
+        <v>4700001</v>
+      </c>
+      <c r="C77">
+        <v>4739000</v>
+      </c>
+      <c r="D77">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="E77">
+        <f>C77-B77</f>
+        <v>38999</v>
+      </c>
+      <c r="F77" s="4">
+        <f>E77*D77</f>
+        <v>272.99299999999999</v>
+      </c>
+      <c r="G77" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>28</v>
+      </c>
+      <c r="B78">
+        <v>907000</v>
+      </c>
+      <c r="C78">
+        <v>930000</v>
+      </c>
+      <c r="D78">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="E78">
+        <f>C78-B78</f>
+        <v>23000</v>
+      </c>
+      <c r="F78" s="4">
+        <f>E78*D78</f>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>66</v>
+      </c>
+      <c r="B79">
+        <v>1664</v>
+      </c>
+      <c r="C79">
+        <v>1681</v>
+      </c>
+      <c r="D79">
+        <v>7.5</v>
+      </c>
+      <c r="E79">
+        <f>C79-B79</f>
+        <v>17</v>
+      </c>
+      <c r="F79" s="4">
+        <f>E79*D79</f>
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>40</v>
+      </c>
+      <c r="B80">
+        <v>885900</v>
+      </c>
+      <c r="C80">
+        <v>905000</v>
+      </c>
+      <c r="D80">
+        <v>1.4E-2</v>
+      </c>
+      <c r="E80">
+        <f>C80-B80</f>
+        <v>19100</v>
+      </c>
+      <c r="F80" s="4">
+        <f>E80*D80</f>
+        <v>267.39999999999998</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>57</v>
+      </c>
+      <c r="B81">
+        <v>4131563</v>
+      </c>
+      <c r="C81">
+        <v>4192000</v>
+      </c>
+      <c r="D81">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="E81">
+        <f>C81-B81</f>
+        <v>60437</v>
+      </c>
+      <c r="F81" s="4">
+        <f>E81*D81</f>
+        <v>423.05900000000003</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>67</v>
+      </c>
+      <c r="B82">
+        <v>735001</v>
+      </c>
+      <c r="C82">
+        <v>759011</v>
+      </c>
+      <c r="D82">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="E82">
+        <f>C82-B82</f>
+        <v>24010</v>
+      </c>
+      <c r="F82" s="4">
+        <f>E82*D82</f>
+        <v>168.07</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E83">
+        <f>C83-B83</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E61">
-        <f t="shared" si="6"/>
+      <c r="F83" s="4">
+        <f>E83*D83</f>
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E62">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E63">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E64">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E65">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E66">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E67">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E68">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E69">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E70">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E71">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E72">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E73">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E74">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E75">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E76">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E77">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E78">
-        <f t="shared" ref="E78:E88" si="7">C78-B78</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E79">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E80">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E81">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E82">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E83">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E84">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E85">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E86">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E87">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E88">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="E84" si="7">C84-B84</f>
         <v>0</v>
       </c>
     </row>
@@ -2263,18 +2717,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D75B644-04DB-4EA7-9583-718DDF637643}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -2297,7 +2751,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -2322,7 +2776,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -2347,7 +2801,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2372,7 +2826,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -2397,7 +2851,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -2412,6 +2866,56 @@
       </c>
       <c r="G6" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7">
+        <v>1300</v>
+      </c>
+      <c r="C7">
+        <v>1322</v>
+      </c>
+      <c r="D7">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <f>C7-B7</f>
+        <v>22</v>
+      </c>
+      <c r="F7" s="4">
+        <f>E7*D7</f>
+        <v>198</v>
+      </c>
+      <c r="G7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8">
+        <v>1424</v>
+      </c>
+      <c r="C8">
+        <v>1452</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <f>C8-B8</f>
+        <v>28</v>
+      </c>
+      <c r="F8" s="4">
+        <f>E8*D8</f>
+        <v>280</v>
+      </c>
+      <c r="G8" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated TODO, minor tweaks
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\file_sys\work\workspace\osrs_stocks_12_3\osrs_stocks-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\file_sys\work\workspace\osrs_stocks_12_9\osrs_stocks-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68546567-1761-4FA4-9E38-B61EF65DD918}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E57FF4-E333-4158-9345-EEE76CCD5A17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47880" yWindow="2655" windowWidth="24240" windowHeight="13140" xr2:uid="{3A4BCD19-BC7F-46D6-80EE-26271915C7B0}"/>
+    <workbookView xWindow="-32820" yWindow="-2775" windowWidth="13740" windowHeight="23640" xr2:uid="{3A4BCD19-BC7F-46D6-80EE-26271915C7B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="68">
   <si>
     <t>Shark</t>
   </si>
@@ -610,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAF0EA10-1A19-4FED-AAA3-974607F1F301}">
-  <dimension ref="A1:M84"/>
+  <dimension ref="A1:M123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H91" sqref="H91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,8 +788,8 @@
         <v>19</v>
       </c>
       <c r="H5">
-        <f>SUM(F2:F94)</f>
-        <v>17549.015000000003</v>
+        <f>SUM(F2:F91)</f>
+        <v>20293.902999999998</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1535,7 +1535,7 @@
         <v>28996</v>
       </c>
       <c r="F35" s="4">
-        <f t="shared" ref="F35:F58" si="5">E35*D35</f>
+        <f t="shared" ref="F35:F57" si="5">E35*D35</f>
         <v>202.97200000000001</v>
       </c>
       <c r="G35" t="s">
@@ -1881,7 +1881,7 @@
         <v>7.5</v>
       </c>
       <c r="E49">
-        <f t="shared" ref="E49:E58" si="6">C49-B49</f>
+        <f t="shared" ref="E49:E57" si="6">C49-B49</f>
         <v>34</v>
       </c>
       <c r="F49" s="4">
@@ -2094,72 +2094,75 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="B58">
-        <v>1248</v>
+        <v>6107000</v>
       </c>
       <c r="C58">
-        <v>1274</v>
+        <v>6376000</v>
       </c>
       <c r="D58">
-        <v>11</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="E58">
-        <f t="shared" si="6"/>
-        <v>26</v>
+        <f t="shared" ref="E58:E80" si="7">C58-B58</f>
+        <v>269000</v>
       </c>
       <c r="F58" s="4">
-        <f t="shared" si="5"/>
-        <v>286</v>
-      </c>
+        <f t="shared" ref="F58:F80" si="8">E58*D58</f>
+        <v>807</v>
+      </c>
+      <c r="G58" t="s">
+        <v>19</v>
+      </c>
+      <c r="H58" s="4"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B59">
-        <v>6107000</v>
+        <v>1825</v>
       </c>
       <c r="C59">
-        <v>6376000</v>
+        <v>1990</v>
       </c>
       <c r="D59">
-        <v>3.0000000000000001E-3</v>
+        <v>0.2</v>
       </c>
       <c r="E59">
-        <f>C59-B59</f>
-        <v>269000</v>
+        <f t="shared" si="7"/>
+        <v>165</v>
       </c>
       <c r="F59" s="4">
-        <f>E59*D59</f>
-        <v>807</v>
+        <f t="shared" si="8"/>
+        <v>33</v>
       </c>
       <c r="G59" t="s">
         <v>19</v>
       </c>
-      <c r="H59" s="4"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B60">
-        <v>1825</v>
+        <v>7800</v>
       </c>
       <c r="C60">
-        <v>1990</v>
+        <v>9000</v>
       </c>
       <c r="D60">
-        <v>0.2</v>
+        <v>0.12</v>
       </c>
       <c r="E60">
-        <f>C60-B60</f>
-        <v>165</v>
+        <f t="shared" si="7"/>
+        <v>1200</v>
       </c>
       <c r="F60" s="4">
-        <f>E60*D60</f>
-        <v>33</v>
+        <f t="shared" si="8"/>
+        <v>144</v>
       </c>
       <c r="G60" t="s">
         <v>19</v>
@@ -2167,24 +2170,24 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B61">
-        <v>7800</v>
+        <v>405000</v>
       </c>
       <c r="C61">
-        <v>9000</v>
+        <v>412000</v>
       </c>
       <c r="D61">
-        <v>0.12</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="E61">
-        <f>C61-B61</f>
-        <v>1200</v>
+        <f t="shared" si="7"/>
+        <v>7000</v>
       </c>
       <c r="F61" s="4">
-        <f>E61*D61</f>
-        <v>144</v>
+        <f t="shared" si="8"/>
+        <v>245.00000000000003</v>
       </c>
       <c r="G61" t="s">
         <v>19</v>
@@ -2192,24 +2195,24 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B62">
-        <v>405000</v>
+        <v>2745</v>
       </c>
       <c r="C62">
-        <v>412000</v>
+        <v>2990</v>
       </c>
       <c r="D62">
-        <v>3.5000000000000003E-2</v>
+        <v>2</v>
       </c>
       <c r="E62">
-        <f>C62-B62</f>
-        <v>7000</v>
+        <f t="shared" si="7"/>
+        <v>245</v>
       </c>
       <c r="F62" s="4">
-        <f>E62*D62</f>
-        <v>245.00000000000003</v>
+        <f t="shared" si="8"/>
+        <v>490</v>
       </c>
       <c r="G62" t="s">
         <v>19</v>
@@ -2217,24 +2220,24 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B63">
-        <v>2745</v>
+        <v>4512000</v>
       </c>
       <c r="C63">
-        <v>2990</v>
+        <v>4650000</v>
       </c>
       <c r="D63">
-        <v>2</v>
+        <v>2E-3</v>
       </c>
       <c r="E63">
-        <f>C63-B63</f>
-        <v>245</v>
+        <f t="shared" si="7"/>
+        <v>138000</v>
       </c>
       <c r="F63" s="4">
-        <f>E63*D63</f>
-        <v>490</v>
+        <f t="shared" si="8"/>
+        <v>276</v>
       </c>
       <c r="G63" t="s">
         <v>19</v>
@@ -2242,24 +2245,24 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B64">
-        <v>4512000</v>
+        <v>627</v>
       </c>
       <c r="C64">
-        <v>4650000</v>
+        <v>640</v>
       </c>
       <c r="D64">
-        <v>2E-3</v>
+        <v>10</v>
       </c>
       <c r="E64">
-        <f>C64-B64</f>
-        <v>138000</v>
+        <f t="shared" si="7"/>
+        <v>13</v>
       </c>
       <c r="F64" s="4">
-        <f>E64*D64</f>
-        <v>276</v>
+        <f t="shared" si="8"/>
+        <v>130</v>
       </c>
       <c r="G64" t="s">
         <v>19</v>
@@ -2267,24 +2270,24 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B65">
-        <v>627</v>
+        <v>4021000</v>
       </c>
       <c r="C65">
-        <v>640</v>
+        <v>4084990</v>
       </c>
       <c r="D65">
-        <v>10</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="E65">
-        <f>C65-B65</f>
-        <v>13</v>
+        <f t="shared" si="7"/>
+        <v>63990</v>
       </c>
       <c r="F65" s="4">
-        <f>E65*D65</f>
-        <v>130</v>
+        <f t="shared" si="8"/>
+        <v>447.93</v>
       </c>
       <c r="G65" t="s">
         <v>19</v>
@@ -2292,24 +2295,24 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B66">
-        <v>4021000</v>
+        <v>4680</v>
       </c>
       <c r="C66">
-        <v>4084990</v>
+        <v>4722</v>
       </c>
       <c r="D66">
-        <v>7.0000000000000001E-3</v>
+        <v>2</v>
       </c>
       <c r="E66">
-        <f>C66-B66</f>
-        <v>63990</v>
+        <f t="shared" si="7"/>
+        <v>42</v>
       </c>
       <c r="F66" s="4">
-        <f>E66*D66</f>
-        <v>447.93</v>
+        <f t="shared" si="8"/>
+        <v>84</v>
       </c>
       <c r="G66" t="s">
         <v>19</v>
@@ -2317,24 +2320,24 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B67">
-        <v>4680</v>
+        <v>487199</v>
       </c>
       <c r="C67">
-        <v>4722</v>
+        <v>512400</v>
       </c>
       <c r="D67">
-        <v>2</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="E67">
-        <f>C67-B67</f>
-        <v>42</v>
+        <f t="shared" si="7"/>
+        <v>25201</v>
       </c>
       <c r="F67" s="4">
-        <f>E67*D67</f>
-        <v>84</v>
+        <f t="shared" si="8"/>
+        <v>176.40700000000001</v>
       </c>
       <c r="G67" t="s">
         <v>19</v>
@@ -2342,24 +2345,24 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="B68">
-        <v>487199</v>
+        <v>45650</v>
       </c>
       <c r="C68">
-        <v>512400</v>
+        <v>47650</v>
       </c>
       <c r="D68">
-        <v>7.0000000000000001E-3</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E68">
-        <f>C68-B68</f>
-        <v>25201</v>
+        <f t="shared" si="7"/>
+        <v>2000</v>
       </c>
       <c r="F68" s="4">
-        <f>E68*D68</f>
-        <v>176.40700000000001</v>
+        <f t="shared" si="8"/>
+        <v>140</v>
       </c>
       <c r="G68" t="s">
         <v>19</v>
@@ -2367,24 +2370,24 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B69">
-        <v>45650</v>
+        <v>3022</v>
       </c>
       <c r="C69">
-        <v>47650</v>
+        <v>3045</v>
       </c>
       <c r="D69">
-        <v>7.0000000000000007E-2</v>
+        <v>7.5</v>
       </c>
       <c r="E69">
-        <f>C69-B69</f>
-        <v>2000</v>
+        <f t="shared" si="7"/>
+        <v>23</v>
       </c>
       <c r="F69" s="4">
-        <f>E69*D69</f>
-        <v>140</v>
+        <f t="shared" si="8"/>
+        <v>172.5</v>
       </c>
       <c r="G69" t="s">
         <v>19</v>
@@ -2392,24 +2395,24 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B70">
-        <v>3022</v>
+        <v>235</v>
       </c>
       <c r="C70">
-        <v>3045</v>
+        <v>237</v>
       </c>
       <c r="D70">
-        <v>7.5</v>
+        <v>30</v>
       </c>
       <c r="E70">
-        <f>C70-B70</f>
-        <v>23</v>
+        <f t="shared" si="7"/>
+        <v>2</v>
       </c>
       <c r="F70" s="4">
-        <f>E70*D70</f>
-        <v>172.5</v>
+        <f t="shared" si="8"/>
+        <v>60</v>
       </c>
       <c r="G70" t="s">
         <v>19</v>
@@ -2417,24 +2420,24 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B71">
-        <v>235</v>
+        <v>894000</v>
       </c>
       <c r="C71">
-        <v>237</v>
+        <v>944500</v>
       </c>
       <c r="D71">
-        <v>30</v>
+        <v>2E-3</v>
       </c>
       <c r="E71">
-        <f>C71-B71</f>
-        <v>2</v>
+        <f t="shared" si="7"/>
+        <v>50500</v>
       </c>
       <c r="F71" s="4">
-        <f>E71*D71</f>
-        <v>60</v>
+        <f t="shared" si="8"/>
+        <v>101</v>
       </c>
       <c r="G71" t="s">
         <v>19</v>
@@ -2442,24 +2445,24 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="B72">
-        <v>894000</v>
+        <v>1030000</v>
       </c>
       <c r="C72">
-        <v>944500</v>
+        <v>1040000</v>
       </c>
       <c r="D72">
-        <v>2E-3</v>
+        <v>1.4E-2</v>
       </c>
       <c r="E72">
-        <f>C72-B72</f>
-        <v>50500</v>
+        <f t="shared" si="7"/>
+        <v>10000</v>
       </c>
       <c r="F72" s="4">
-        <f>E72*D72</f>
-        <v>101</v>
+        <f t="shared" si="8"/>
+        <v>140</v>
       </c>
       <c r="G72" t="s">
         <v>19</v>
@@ -2467,24 +2470,24 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="B73">
-        <v>1030000</v>
+        <v>6180000</v>
       </c>
       <c r="C73">
-        <v>1040000</v>
+        <v>6350000</v>
       </c>
       <c r="D73">
-        <v>1.4E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="E73">
-        <f>C73-B73</f>
-        <v>10000</v>
+        <f t="shared" si="7"/>
+        <v>170000</v>
       </c>
       <c r="F73" s="4">
-        <f>E73*D73</f>
-        <v>140</v>
+        <f t="shared" si="8"/>
+        <v>680</v>
       </c>
       <c r="G73" t="s">
         <v>19</v>
@@ -2492,46 +2495,49 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B74">
-        <v>6180000</v>
+        <v>633</v>
       </c>
       <c r="C74">
-        <v>6350000</v>
+        <v>640</v>
       </c>
       <c r="D74">
-        <v>8.0000000000000002E-3</v>
+        <v>10</v>
       </c>
       <c r="E74">
-        <f>C74-B74</f>
-        <v>170000</v>
+        <f t="shared" si="7"/>
+        <v>7</v>
       </c>
       <c r="F74" s="4">
-        <f>E74*D74</f>
-        <v>1360</v>
+        <f t="shared" si="8"/>
+        <v>70</v>
+      </c>
+      <c r="G74" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B75">
-        <v>633</v>
+        <v>2659</v>
       </c>
       <c r="C75">
-        <v>640</v>
+        <v>2747</v>
       </c>
       <c r="D75">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E75">
-        <f>C75-B75</f>
-        <v>7</v>
+        <f t="shared" si="7"/>
+        <v>88</v>
       </c>
       <c r="F75" s="4">
-        <f>E75*D75</f>
-        <v>70</v>
+        <f t="shared" si="8"/>
+        <v>176</v>
       </c>
       <c r="G75" t="s">
         <v>19</v>
@@ -2539,46 +2545,49 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="B76">
-        <v>2659</v>
+        <v>4700001</v>
       </c>
       <c r="C76">
-        <v>2747</v>
+        <v>4739000</v>
       </c>
       <c r="D76">
-        <v>2</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="E76">
-        <f>C76-B76</f>
-        <v>88</v>
+        <f t="shared" si="7"/>
+        <v>38999</v>
       </c>
       <c r="F76" s="4">
-        <f>E76*D76</f>
-        <v>176</v>
+        <f t="shared" si="8"/>
+        <v>272.99299999999999</v>
+      </c>
+      <c r="G76" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="B77">
-        <v>4700001</v>
+        <v>907000</v>
       </c>
       <c r="C77">
-        <v>4739000</v>
+        <v>919000</v>
       </c>
       <c r="D77">
-        <v>7.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E77">
-        <f>C77-B77</f>
-        <v>38999</v>
+        <f t="shared" si="7"/>
+        <v>12000</v>
       </c>
       <c r="F77" s="4">
-        <f>E77*D77</f>
-        <v>272.99299999999999</v>
+        <f t="shared" si="8"/>
+        <v>60</v>
       </c>
       <c r="G77" t="s">
         <v>19</v>
@@ -2586,127 +2595,920 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="B78">
-        <v>907000</v>
+        <v>1664</v>
       </c>
       <c r="C78">
-        <v>930000</v>
+        <v>1680</v>
       </c>
       <c r="D78">
-        <v>7.0000000000000001E-3</v>
+        <v>7.5</v>
       </c>
       <c r="E78">
-        <f>C78-B78</f>
-        <v>23000</v>
+        <f t="shared" si="7"/>
+        <v>16</v>
       </c>
       <c r="F78" s="4">
-        <f>E78*D78</f>
-        <v>161</v>
+        <f t="shared" si="8"/>
+        <v>120</v>
+      </c>
+      <c r="G78" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B79">
-        <v>1664</v>
+        <v>4131563</v>
       </c>
       <c r="C79">
-        <v>1681</v>
+        <v>4192000</v>
       </c>
       <c r="D79">
-        <v>7.5</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="E79">
-        <f>C79-B79</f>
-        <v>17</v>
+        <f t="shared" si="7"/>
+        <v>60437</v>
       </c>
       <c r="F79" s="4">
-        <f>E79*D79</f>
-        <v>127.5</v>
+        <f t="shared" si="8"/>
+        <v>423.05900000000003</v>
+      </c>
+      <c r="G79" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>67</v>
+      </c>
+      <c r="B80">
+        <v>735001</v>
+      </c>
+      <c r="C80">
+        <v>753000</v>
+      </c>
+      <c r="D80">
+        <v>2E-3</v>
+      </c>
+      <c r="E80">
+        <f t="shared" si="7"/>
+        <v>17999</v>
+      </c>
+      <c r="F80" s="4">
+        <f t="shared" si="8"/>
+        <v>35.997999999999998</v>
+      </c>
+      <c r="G80" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>25</v>
+      </c>
+      <c r="B81">
+        <v>301</v>
+      </c>
+      <c r="C81">
+        <v>305</v>
+      </c>
+      <c r="D81">
+        <v>10</v>
+      </c>
+      <c r="E81">
+        <f t="shared" ref="E81:E86" si="9">C81-B81</f>
+        <v>4</v>
+      </c>
+      <c r="F81" s="4">
+        <f t="shared" ref="F81:F86" si="10">E81*D81</f>
         <v>40</v>
       </c>
-      <c r="B80">
-        <v>885900</v>
-      </c>
-      <c r="C80">
-        <v>905000</v>
-      </c>
-      <c r="D80">
-        <v>1.4E-2</v>
-      </c>
-      <c r="E80">
-        <f>C80-B80</f>
-        <v>19100</v>
-      </c>
-      <c r="F80" s="4">
-        <f>E80*D80</f>
-        <v>267.39999999999998</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="G81" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>20</v>
+      </c>
+      <c r="B82">
+        <v>1737</v>
+      </c>
+      <c r="C82">
+        <v>1765</v>
+      </c>
+      <c r="D82">
+        <v>10</v>
+      </c>
+      <c r="E82">
+        <f t="shared" si="9"/>
+        <v>28</v>
+      </c>
+      <c r="F82" s="4">
+        <f t="shared" si="10"/>
+        <v>280</v>
+      </c>
+      <c r="G82" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>16</v>
+      </c>
+      <c r="B83">
+        <v>3012</v>
+      </c>
+      <c r="C83">
+        <v>3052</v>
+      </c>
+      <c r="D83">
+        <v>7.5</v>
+      </c>
+      <c r="E83">
+        <f t="shared" si="9"/>
+        <v>40</v>
+      </c>
+      <c r="F83" s="4">
+        <f t="shared" si="10"/>
+        <v>300</v>
+      </c>
+      <c r="G83" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>17</v>
+      </c>
+      <c r="B84">
+        <v>237</v>
+      </c>
+      <c r="C84">
+        <v>240</v>
+      </c>
+      <c r="D84">
+        <v>30</v>
+      </c>
+      <c r="E84">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="F84" s="4">
+        <f t="shared" si="10"/>
+        <v>90</v>
+      </c>
+      <c r="G84" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>61</v>
+      </c>
+      <c r="B85">
+        <v>401001</v>
+      </c>
+      <c r="C85">
+        <v>414399</v>
+      </c>
+      <c r="D85">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E85">
+        <f t="shared" si="9"/>
+        <v>13398</v>
+      </c>
+      <c r="F85" s="4">
+        <f t="shared" si="10"/>
+        <v>937.86000000000013</v>
+      </c>
+      <c r="G85" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>16</v>
+      </c>
+      <c r="B86">
+        <v>3032</v>
+      </c>
+      <c r="C86">
+        <v>3101</v>
+      </c>
+      <c r="D86">
+        <v>6.5</v>
+      </c>
+      <c r="E86">
+        <f t="shared" si="9"/>
+        <v>69</v>
+      </c>
+      <c r="F86" s="4">
+        <f t="shared" si="10"/>
+        <v>448.5</v>
+      </c>
+      <c r="G86" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>66</v>
+      </c>
+      <c r="B87">
+        <v>1605</v>
+      </c>
+      <c r="C87">
+        <v>1670</v>
+      </c>
+      <c r="D87">
+        <v>7.5</v>
+      </c>
+      <c r="E87">
+        <f t="shared" ref="E87:E100" si="11">C87-B87</f>
+        <v>65</v>
+      </c>
+      <c r="F87" s="4">
+        <f t="shared" ref="F87:F100" si="12">E87*D87</f>
+        <v>487.5</v>
+      </c>
+      <c r="G87" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>57</v>
       </c>
-      <c r="B81">
-        <v>4131563</v>
-      </c>
-      <c r="C81">
-        <v>4192000</v>
-      </c>
-      <c r="D81">
+      <c r="B88">
+        <v>4064000</v>
+      </c>
+      <c r="C88">
+        <v>4075000</v>
+      </c>
+      <c r="D88">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="E81">
-        <f>C81-B81</f>
-        <v>60437</v>
-      </c>
-      <c r="F81" s="4">
-        <f>E81*D81</f>
-        <v>423.05900000000003</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>67</v>
-      </c>
-      <c r="B82">
-        <v>735001</v>
-      </c>
-      <c r="C82">
-        <v>759011</v>
-      </c>
-      <c r="D82">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="E82">
-        <f>C82-B82</f>
-        <v>24010</v>
-      </c>
-      <c r="F82" s="4">
-        <f>E82*D82</f>
-        <v>168.07</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E83">
-        <f>C83-B83</f>
+      <c r="E88">
+        <f t="shared" si="11"/>
+        <v>11000</v>
+      </c>
+      <c r="F88" s="4">
+        <f t="shared" si="12"/>
+        <v>77</v>
+      </c>
+      <c r="G88" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>45</v>
+      </c>
+      <c r="B89">
+        <v>2651</v>
+      </c>
+      <c r="C89">
+        <v>2709</v>
+      </c>
+      <c r="D89">
+        <v>2</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="11"/>
+        <v>58</v>
+      </c>
+      <c r="F89" s="4">
+        <f t="shared" si="12"/>
+        <v>116</v>
+      </c>
+      <c r="G89" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>38</v>
+      </c>
+      <c r="B90">
+        <v>245</v>
+      </c>
+      <c r="C90">
+        <v>252</v>
+      </c>
+      <c r="D90">
+        <v>30</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="11"/>
+        <v>7</v>
+      </c>
+      <c r="F90" s="4">
+        <f t="shared" si="12"/>
+        <v>210</v>
+      </c>
+      <c r="G90" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>65</v>
+      </c>
+      <c r="B91">
+        <v>4892000</v>
+      </c>
+      <c r="C91">
+        <v>5200000</v>
+      </c>
+      <c r="D91">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="11"/>
+        <v>308000</v>
+      </c>
+      <c r="F91" s="4">
+        <f t="shared" si="12"/>
+        <v>1232</v>
+      </c>
+      <c r="G91" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>61</v>
+      </c>
+      <c r="B92">
+        <v>405000</v>
+      </c>
+      <c r="C92">
+        <v>410000</v>
+      </c>
+      <c r="D92">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="E92">
+        <f t="shared" si="11"/>
+        <v>5000</v>
+      </c>
+      <c r="F92" s="4">
+        <f t="shared" si="12"/>
+        <v>175.00000000000003</v>
+      </c>
+      <c r="G92" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>20</v>
+      </c>
+      <c r="B93">
+        <v>1674</v>
+      </c>
+      <c r="C93">
+        <v>1690</v>
+      </c>
+      <c r="D93">
+        <v>7</v>
+      </c>
+      <c r="E93">
+        <f t="shared" si="11"/>
+        <v>16</v>
+      </c>
+      <c r="F93" s="4">
+        <f t="shared" si="12"/>
+        <v>112</v>
+      </c>
+      <c r="G93" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>58</v>
+      </c>
+      <c r="B94">
+        <v>621</v>
+      </c>
+      <c r="C94">
+        <v>628</v>
+      </c>
+      <c r="D94">
+        <v>10</v>
+      </c>
+      <c r="E94">
+        <f t="shared" si="11"/>
+        <v>7</v>
+      </c>
+      <c r="F94" s="4">
+        <f t="shared" si="12"/>
+        <v>70</v>
+      </c>
+      <c r="G94" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>56</v>
+      </c>
+      <c r="B95">
+        <v>4663</v>
+      </c>
+      <c r="C95">
+        <v>4699</v>
+      </c>
+      <c r="D95">
+        <v>2</v>
+      </c>
+      <c r="E95">
+        <f t="shared" si="11"/>
+        <v>36</v>
+      </c>
+      <c r="F95" s="4">
+        <f t="shared" si="12"/>
+        <v>72</v>
+      </c>
+      <c r="G95" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>47</v>
+      </c>
+      <c r="B96">
+        <v>986</v>
+      </c>
+      <c r="C96">
+        <v>1020</v>
+      </c>
+      <c r="D96">
+        <v>11</v>
+      </c>
+      <c r="E96">
+        <f t="shared" si="11"/>
+        <v>34</v>
+      </c>
+      <c r="F96" s="4">
+        <f t="shared" si="12"/>
+        <v>374</v>
+      </c>
+      <c r="G96" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>16</v>
+      </c>
+      <c r="B97">
+        <v>2968</v>
+      </c>
+      <c r="C97">
+        <v>3018</v>
+      </c>
+      <c r="D97">
+        <v>7.5</v>
+      </c>
+      <c r="E97">
+        <f t="shared" si="11"/>
+        <v>50</v>
+      </c>
+      <c r="F97" s="4">
+        <f t="shared" si="12"/>
+        <v>375</v>
+      </c>
+      <c r="G97" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>45</v>
+      </c>
+      <c r="B98">
+        <v>3102</v>
+      </c>
+      <c r="C98">
+        <v>3600</v>
+      </c>
+      <c r="D98">
+        <v>2</v>
+      </c>
+      <c r="E98">
+        <f t="shared" si="11"/>
+        <v>498</v>
+      </c>
+      <c r="F98" s="4">
+        <f t="shared" si="12"/>
+        <v>996</v>
+      </c>
+      <c r="G98" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>49</v>
+      </c>
+      <c r="B99">
+        <v>1003000</v>
+      </c>
+      <c r="C99">
+        <v>1255000</v>
+      </c>
+      <c r="D99">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E99">
+        <f t="shared" si="11"/>
+        <v>252000</v>
+      </c>
+      <c r="F99" s="4">
+        <f t="shared" si="12"/>
+        <v>1008</v>
+      </c>
+      <c r="G99" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>64</v>
+      </c>
+      <c r="B100">
+        <v>6010000</v>
+      </c>
+      <c r="C100">
+        <v>6230000</v>
+      </c>
+      <c r="D100">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E100">
+        <f t="shared" si="11"/>
+        <v>220000</v>
+      </c>
+      <c r="F100" s="4">
+        <f t="shared" si="12"/>
+        <v>880</v>
+      </c>
+      <c r="G100" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>58</v>
+      </c>
+      <c r="B101">
+        <v>620</v>
+      </c>
+      <c r="C101">
+        <v>627</v>
+      </c>
+      <c r="D101">
+        <v>7</v>
+      </c>
+      <c r="E101">
+        <f t="shared" ref="E101:E123" si="13">C101-B101</f>
+        <v>7</v>
+      </c>
+      <c r="F101" s="4">
+        <f t="shared" ref="F101:F123" si="14">E101*D101</f>
+        <v>49</v>
+      </c>
+      <c r="G101" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>65</v>
+      </c>
+      <c r="B102">
+        <v>4892000</v>
+      </c>
+      <c r="C102">
+        <v>5050000</v>
+      </c>
+      <c r="D102">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E102">
+        <f t="shared" si="13"/>
+        <v>158000</v>
+      </c>
+      <c r="F102" s="4">
+        <f t="shared" si="14"/>
+        <v>474</v>
+      </c>
+      <c r="G102" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>61</v>
+      </c>
+      <c r="B103">
+        <v>409000</v>
+      </c>
+      <c r="C103">
+        <v>425000</v>
+      </c>
+      <c r="D103">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E103">
+        <f t="shared" si="13"/>
+        <v>16000</v>
+      </c>
+      <c r="F103" s="4">
+        <f t="shared" si="14"/>
+        <v>1120</v>
+      </c>
+      <c r="G103" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>48</v>
+      </c>
+      <c r="B104">
+        <v>1480</v>
+      </c>
+      <c r="C104">
+        <v>1494</v>
+      </c>
+      <c r="D104">
+        <v>10</v>
+      </c>
+      <c r="E104">
+        <f t="shared" si="13"/>
+        <v>14</v>
+      </c>
+      <c r="F104" s="4">
+        <f t="shared" si="14"/>
+        <v>140</v>
+      </c>
+      <c r="G104" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>45</v>
+      </c>
+      <c r="B105">
+        <v>2850</v>
+      </c>
+      <c r="C105">
+        <v>3120</v>
+      </c>
+      <c r="D105">
+        <v>2</v>
+      </c>
+      <c r="E105">
+        <f t="shared" si="13"/>
+        <v>270</v>
+      </c>
+      <c r="F105" s="4">
+        <f t="shared" si="14"/>
+        <v>540</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>56</v>
+      </c>
+      <c r="B106">
+        <v>4647</v>
+      </c>
+      <c r="C106">
+        <v>4718</v>
+      </c>
+      <c r="D106">
+        <v>2</v>
+      </c>
+      <c r="E106">
+        <f t="shared" si="13"/>
+        <v>71</v>
+      </c>
+      <c r="F106" s="4">
+        <f t="shared" si="14"/>
+        <v>142</v>
+      </c>
+      <c r="G106" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>36</v>
+      </c>
+      <c r="B107">
+        <v>2954</v>
+      </c>
+      <c r="C107">
+        <v>2990</v>
+      </c>
+      <c r="D107">
+        <v>7.5</v>
+      </c>
+      <c r="E107">
+        <f t="shared" si="13"/>
+        <v>36</v>
+      </c>
+      <c r="F107" s="4">
+        <f t="shared" si="14"/>
+        <v>270</v>
+      </c>
+      <c r="G107" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>36</v>
+      </c>
+      <c r="B108">
+        <v>2910</v>
+      </c>
+      <c r="C108">
+        <v>2963</v>
+      </c>
+      <c r="D108">
+        <v>7.5</v>
+      </c>
+      <c r="E108">
+        <f t="shared" si="13"/>
+        <v>53</v>
+      </c>
+      <c r="F108" s="4">
+        <f t="shared" si="14"/>
+        <v>397.5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E109">
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="F83" s="4">
-        <f>E83*D83</f>
+      <c r="F109" s="4">
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E84">
-        <f t="shared" ref="E84" si="7">C84-B84</f>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E110">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="F110" s="4">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E111">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="F111" s="4">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E112">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="F112" s="4">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E113">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="F113" s="4">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E114">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="F114" s="4">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E115">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="F115" s="4">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E116">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="F116" s="4">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E117">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="F117" s="4">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E118">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="F118" s="4">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E119">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="F119" s="4">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E120">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="F120" s="4">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E121">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="F121" s="4">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E122">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="F122" s="4">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E123">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="F123" s="4">
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>